<commit_message>
drop down and graphs
</commit_message>
<xml_diff>
--- a/kobo_forms/form_meta_fr.xlsx
+++ b/kobo_forms/form_meta_fr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4eeea2119f37a1e9/My Documents/Websites/mada_whale/kobo_forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{30934CAC-07B5-4941-BABD-97AFD8560660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B135A48-70F8-4C96-91AE-B5C18F8C3D14}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{30934CAC-07B5-4941-BABD-97AFD8560660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4B06DD4-FECA-4162-9BE7-1462F56033D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{F868EB87-613D-4D57-84C6-7576153D1BEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{F868EB87-613D-4D57-84C6-7576153D1BEA}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="363">
   <si>
     <t>type</t>
   </si>
@@ -66,34 +66,7 @@
     <t>research</t>
   </si>
   <si>
-    <t>select_one guide</t>
-  </si>
-  <si>
     <t>guide</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>paul</t>
-  </si>
-  <si>
-    <t>george</t>
-  </si>
-  <si>
-    <t>ringo</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Ringo</t>
   </si>
   <si>
     <t>observer</t>
@@ -344,9 +317,6 @@
     <t>Faux Orque</t>
   </si>
   <si>
-    <t>autres_espece</t>
-  </si>
-  <si>
     <t>baleine_bosse</t>
   </si>
   <si>
@@ -398,9 +368,6 @@
     <t>${trichodesmium}='yes'</t>
   </si>
   <si>
-    <t>gps</t>
-  </si>
-  <si>
     <t>select_one sex</t>
   </si>
   <si>
@@ -944,9 +911,6 @@
     <t xml:space="preserve">Photo d'identification droite? </t>
   </si>
   <si>
-    <t>Placement GPS</t>
-  </si>
-  <si>
     <t>Sexe</t>
   </si>
   <si>
@@ -1079,9 +1043,6 @@
     <t>Autre mégafaune</t>
   </si>
   <si>
-    <t>Autres Espèces</t>
-  </si>
-  <si>
     <t>Mâle</t>
   </si>
   <si>
@@ -1095,9 +1056,6 @@
   </si>
   <si>
     <t>(. &gt;=25 and .&lt;=35)</t>
-  </si>
-  <si>
-    <t>GPS placeholder</t>
   </si>
   <si>
     <t>(${left_id}='yes') and (${operator} = 'research')</t>
@@ -1124,6 +1082,63 @@
   <si>
     <t>Recontre ajoutée! 
 Passer au suivant, si observé.</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>megaf_geo</t>
+  </si>
+  <si>
+    <t>Coordonnées gps d'observation</t>
+  </si>
+  <si>
+    <t>shark_geo</t>
+  </si>
+  <si>
+    <t>Press save before 5m</t>
+  </si>
+  <si>
+    <t>demi</t>
+  </si>
+  <si>
+    <t>Demi</t>
+  </si>
+  <si>
+    <t>grand_dauphin</t>
+  </si>
+  <si>
+    <t>Grand Dauphin</t>
+  </si>
+  <si>
+    <t>dauphin</t>
+  </si>
+  <si>
+    <t>Dauphin</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Emilie</t>
+  </si>
+  <si>
+    <t>Tanguy</t>
+  </si>
+  <si>
+    <t>Elina</t>
+  </si>
+  <si>
+    <t>Elise</t>
+  </si>
+  <si>
+    <t>Guillaume</t>
+  </si>
+  <si>
+    <t>select_one guide or_other</t>
   </si>
 </sst>
 </file>
@@ -1509,11 +1524,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7AE5F8-6897-4EA6-B848-F71675BD52F0}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,43 +1557,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F2" s="4"/>
       <c r="H2" s="4"/>
@@ -1588,10 +1603,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1"/>
       <c r="F3" s="4"/>
@@ -1602,10 +1617,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="4"/>
@@ -1616,10 +1631,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1"/>
       <c r="F5" s="4"/>
@@ -1630,13 +1645,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F6" s="4"/>
       <c r="H6" s="4"/>
@@ -1646,19 +1661,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1669,919 +1684,925 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>344</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
+      </c>
+      <c r="C20" t="s">
+        <v>346</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>116</v>
+      <c r="A26" t="s">
+        <v>344</v>
+      </c>
+      <c r="B26" t="s">
+        <v>347</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
       <c r="D26" s="3"/>
       <c r="H26" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="D31" s="3"/>
       <c r="H31" s="2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D34" s="3"/>
       <c r="F34" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D41" s="3"/>
       <c r="F41" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="D42" s="3"/>
       <c r="H42" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D43" s="3"/>
       <c r="H43" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="D44" s="3"/>
       <c r="F44" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="D45" s="3"/>
       <c r="H45" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="D46" s="3"/>
       <c r="H46" s="2" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>325</v>
-      </c>
       <c r="H47" s="2" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="D48" s="3"/>
       <c r="H48" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="D49" s="3"/>
       <c r="H49" s="2" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="D50" s="3"/>
       <c r="H50" s="2" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="D51" s="3"/>
       <c r="H51" s="2" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="D52" s="3"/>
       <c r="H52" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="D53" s="3"/>
       <c r="H53" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="D54" s="3"/>
       <c r="H54" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>2</v>
@@ -2589,86 +2610,86 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2679,10 +2700,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1785AC80-7F5A-4FB1-94A5-139ABE7C7498}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2723,1085 +2744,1140 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>355</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>356</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>357</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>358</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>359</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>360</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>361</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>354</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>355</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>336</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>337</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>349</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>340</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>275</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>276</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>275</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>264</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>101</v>
+        <v>265</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>264</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>87</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>352</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>353</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>92</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>343</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>344</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>345</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>346</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>340</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>71</v>
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>128</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>155</v>
+        <v>41</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>129</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>156</v>
+        <v>41</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>157</v>
+        <v>56</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>198</v>
+        <v>158</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>199</v>
+        <v>158</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>70</v>
+      <c r="A81" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>202</v>
+      <c r="A82" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>71</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>207</v>
+      <c r="A83" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>206</v>
+      <c r="A84" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>206</v>
+      <c r="A85" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>215</v>
+        <v>41</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>210</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>216</v>
+        <v>56</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>211</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>50</v>
+        <v>201</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>224</v>
+      <c r="A90" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>229</v>
+        <v>203</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>224</v>
+      <c r="A91" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>224</v>
+      <c r="A92" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>235</v>
+      <c r="A93" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>240</v>
+        <v>41</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>237</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>235</v>
+      <c r="A94" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>241</v>
+        <v>56</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>238</v>
+        <v>62</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>50</v>
+        <v>217</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>71</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>50</v>
+        <v>229</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>70</v>
+        <v>226</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>71</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>50</v>
+        <v>231</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>70</v>
+        <v>228</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>